<commit_message>
Lots of images added and updates to the descriptor file
</commit_message>
<xml_diff>
--- a/pyCybermancy/cybermancy-object-list.xlsx
+++ b/pyCybermancy/cybermancy-object-list.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Daniel\role-gaming\Cybermancy module development\cybermancy\pyCybermancy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\cybermancy\pyCybermancy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590F5681-8598-4824-A1FB-3A8D6F6BA689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39785D1A-5930-428F-A0AA-7341C18D99F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{15A82952-0862-46EA-9957-B8D36A030377}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{15A82952-0862-46EA-9957-B8D36A030377}"/>
   </bookViews>
   <sheets>
     <sheet name="weapons" sheetId="1" r:id="rId1"/>
-    <sheet name="Controlled Lists" sheetId="2" r:id="rId2"/>
-    <sheet name="Actions and Effects" sheetId="3" r:id="rId3"/>
-    <sheet name="Weapon Features" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
+    <sheet name="armor" sheetId="7" r:id="rId2"/>
+    <sheet name="Controlled Lists" sheetId="2" r:id="rId3"/>
+    <sheet name="Actions and Effects" sheetId="3" r:id="rId4"/>
+    <sheet name="Weapon Features" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="1657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4208" uniqueCount="1667">
   <si>
     <t>name</t>
   </si>
@@ -5008,6 +5009,36 @@
   </si>
   <si>
     <t>modules/cybermancy/assets/icons/weapons/emp-singularity.png</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>modules/cybermancy/assets/icons/weapons/fragmentation-grenade-plus.png</t>
+  </si>
+  <si>
+    <t>modules/cybermancy/assets/icons/weapons/emp-grenade-plus.png</t>
+  </si>
+  <si>
+    <t>feature-img</t>
+  </si>
+  <si>
+    <t>critical-effect-img</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Card Name</t>
+  </si>
+  <si>
+    <t>Card Text</t>
+  </si>
+  <si>
+    <t>Card img</t>
+  </si>
+  <si>
+    <t>Hacking</t>
   </si>
 </sst>
 </file>
@@ -5920,7 +5951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8970F5F1-D148-4DDA-AF55-EA0D3E53DF1D}">
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -6848,7 +6879,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1290</v>
       </c>
@@ -8653,6 +8684,3678 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72752D74-2A44-49A3-AA77-657858ABC6FB}">
+  <dimension ref="A1:Z47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="47.26953125" customWidth="1"/>
+    <col min="5" max="5" width="60.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.08984375" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="19.08984375" customWidth="1"/>
+    <col min="21" max="21" width="47.26953125" customWidth="1"/>
+    <col min="22" max="22" width="30.90625" style="4" customWidth="1"/>
+    <col min="23" max="25" width="18.54296875" customWidth="1"/>
+    <col min="26" max="26" width="20.90625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>1611</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>1660</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>1657</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>1612</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>1661</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>1657</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D14" si="0">CONCATENATE("Cybermancy image generator thread: generate an image for ", C2, " in the size recommended by Foundry VTT for icons")</f>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/axes/axe-double-jagged-black.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" t="str">
+        <f>"modules/cybermancy/assets/icons/features/" &amp; LOWER(SUBSTITUTE(S2," ","-"))</f>
+        <v>modules/cybermancy/assets/icons/features/</v>
+      </c>
+      <c r="U2" t="str">
+        <f t="shared" ref="U2:U47" si="1">CONCATENATE("Cybermancy image generator thread: generate an image for ", T2, ".png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by " &amp; S2 &amp; " in the image generation. " &amp; S2 &amp; " in Cybermancy has the effect of: " &amp; V2)</f>
+        <v xml:space="preserve">Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by  in the image generation.  in Cybermancy has the effect of: </v>
+      </c>
+      <c r="X2" t="str">
+        <f>"modules/cybermancy/assets/icons/features/" &amp; LOWER(SUBSTITUTE(W2," ","-"))</f>
+        <v>modules/cybermancy/assets/icons/features/</v>
+      </c>
+      <c r="Y2" t="str">
+        <f t="shared" ref="Y2" si="2">CONCATENATE("Cybermancy image generator thread: generate an image for ", X2, ".png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by " &amp; W2 &amp; " in the image generation. " &amp; W2 &amp; " in Cybermancy has the effect of: " &amp; Z2)</f>
+        <v xml:space="preserve">Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by  in the image generation.  in Cybermancy has the effect of: </v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1614</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/monofilament-whip.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>1557</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1321</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T7" si="3">"modules/cybermancy/assets/icons/features/" &amp; LOWER(SUBSTITUTE(S3," ","-"))</f>
+        <v>modules/cybermancy/assets/icons/features/lethal-edge</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/lethal-edge.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Lethal Edge in the image generation. Lethal Edge in Cybermancy has the effect of:  On a Hope win, deal Severe damage if the Fear die shows 8-12.</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>1398</v>
+      </c>
+      <c r="W3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="X3" t="str">
+        <f t="shared" ref="X3:X47" si="4">"modules/cybermancy/assets/icons/features/" &amp; LOWER(SUBSTITUTE(W3," ","-"))</f>
+        <v>modules/cybermancy/assets/icons/features/slice-in-two</v>
+      </c>
+      <c r="Y3" t="str">
+        <f t="shared" ref="Y3:Y47" si="5">CONCATENATE("Cybermancy image generator thread: generate an image for ", X3, ".png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by " &amp; W3 &amp; " in the image generation. " &amp; W3 &amp; " in Cybermancy has the effect of: " &amp; Z3)</f>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/slice-in-two.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Slice in Two in the image generation. Slice in Two in Cybermancy has the effect of:  Sever or disable a limb, item, or piece of cover.</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/cyber-spur.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>1558</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1267</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1356</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1331</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1399</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="3"/>
+        <v>modules/cybermancy/assets/icons/features/concealed</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/concealed.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Concealed in the image generation. Concealed in Cybermancy has the effect of:  Can be hidden; gain advantage on your first attack each scene.</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>1400</v>
+      </c>
+      <c r="W4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="X4" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/ambush-kill</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/ambush-kill.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Ambush Kill in the image generation. Ambush Kill in Cybermancy has the effect of:  If striking from surprise, escalate Fear consequences for target.</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/shock-baton.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>1559</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1322</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1401</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="3"/>
+        <v>modules/cybermancy/assets/icons/features/stunning</v>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/stunning.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Stunning in the image generation. Stunning in Cybermancy has the effect of:  Spend a Hope on a successful hit to inflict Dazed for one round.</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>1402</v>
+      </c>
+      <c r="W5" t="s">
+        <v>1481</v>
+      </c>
+      <c r="X5" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/knockout</v>
+      </c>
+      <c r="Y5" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/knockout.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Knockout in the image generation. Knockout in Cybermancy has the effect of:  Target is stunned or unconscious for one scene beat.</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1617</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/vibro-knife.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>1560</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1323</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" t="s">
+        <v>1403</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="3"/>
+        <v>modules/cybermancy/assets/icons/features/piercing</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/piercing.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Piercing in the image generation. Piercing in Cybermancy has the effect of:  Ignores armor on a Hope critical.</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>1404</v>
+      </c>
+      <c r="W6" t="s">
+        <v>1483</v>
+      </c>
+      <c r="X6" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/silent-kill</v>
+      </c>
+      <c r="Y6" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/silent-kill.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Silent Kill in the image generation. Silent Kill in Cybermancy has the effect of:  Disable one target silently with no alert escalation.</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1618</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/smartpistol.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>1561</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>1355</v>
+      </c>
+      <c r="P7" t="s">
+        <v>1324</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R7" t="s">
+        <v>25</v>
+      </c>
+      <c r="S7" t="s">
+        <v>1405</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="3"/>
+        <v>modules/cybermancy/assets/icons/features/smartlink</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/smartlink.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Smartlink in the image generation. Smartlink in Cybermancy has the effect of:  Once per scene, reroll one attack die if linked to cyberware/gear.</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>1406</v>
+      </c>
+      <c r="W7" t="s">
+        <v>1485</v>
+      </c>
+      <c r="X7" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/pinpoint</v>
+      </c>
+      <c r="Y7" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/pinpoint.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Pinpoint in the image generation. Pinpoint in Cybermancy has the effect of:  Crit ignores cover; disable weapon/armor.</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1619</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/smg-machine-pistol.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P8" t="s">
+        <v>1325</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1407</v>
+      </c>
+      <c r="T8" t="str">
+        <f>"modules/cybermancy/assets/icons/weapons-feature/" &amp; LOWER(SUBSTITUTE(S8," ","-"))</f>
+        <v>modules/cybermancy/assets/icons/weapons-feature/burst-fire</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/burst-fire.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Burst Fire in the image generation. Burst Fire in Cybermancy has the effect of:  Mark 1 Stress to attack an additional target in Close range.</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>1408</v>
+      </c>
+      <c r="W8" t="s">
+        <v>1487</v>
+      </c>
+      <c r="X8" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/spray-down</v>
+      </c>
+      <c r="Y8" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/spray-down.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Spray Down in the image generation. Spray Down in Cybermancy has the effect of:  Hit all targets in Very Close range with collateral fire.</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/assault-rifle.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>1563</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" t="s">
+        <v>1326</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9" t="s">
+        <v>25</v>
+      </c>
+      <c r="S9" t="s">
+        <v>1409</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" ref="T9:T47" si="6">"modules/cybermancy/assets/icons/weapons-feature/" &amp; LOWER(SUBSTITUTE(S9," ","-"))</f>
+        <v>modules/cybermancy/assets/icons/weapons-feature/suppressive-fire</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/suppressive-fire.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Suppressive Fire in the image generation. Suppressive Fire in Cybermancy has the effect of:  On a Hope win, target must mark 1 Stress to act next turn.</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="W9" t="s">
+        <v>1489</v>
+      </c>
+      <c r="X9" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/shredding-burst</v>
+      </c>
+      <c r="Y9" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/shredding-burst.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Shredding Burst in the image generation. Shredding Burst in Cybermancy has the effect of:  Force enemy into cover, reducing their next attack roll.</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1621</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/shotgun.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>1356</v>
+      </c>
+      <c r="P10" t="s">
+        <v>1327</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>24</v>
+      </c>
+      <c r="R10" t="s">
+        <v>25</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1411</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/scatter</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/scatter.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Scatter in the image generation. Scatter in Cybermancy has the effect of:  Spend a Hope to attack all targets in Very Close range.</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>1412</v>
+      </c>
+      <c r="W10" t="s">
+        <v>1491</v>
+      </c>
+      <c r="X10" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/point-blank-devastation</v>
+      </c>
+      <c r="Y10" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/point-blank-devastation.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Point-Blank Devastation in the image generation. Point-Blank Devastation in Cybermancy has the effect of:  Knock back and lose next action.</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1622</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/sniper-rifle.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>1565</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1354</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1359</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1328</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R11" t="s">
+        <v>25</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1413</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/scoped</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/scoped.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Scoped in the image generation. Scoped in Cybermancy has the effect of:  Spend a round aiming to gain advantage on next shot.</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>1414</v>
+      </c>
+      <c r="W11" t="s">
+        <v>1493</v>
+      </c>
+      <c r="X11" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/through-and-through</v>
+      </c>
+      <c r="Y11" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/through-and-through.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Through and Through in the image generation. Through and Through in Cybermancy has the effect of:  Bullet passes through to a second target in line.</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1623</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/throwing-knives.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>1566</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1329</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S12" t="s">
+        <v>1415</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/quick-draw</v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/quick-draw.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Quick Draw in the image generation. Quick Draw in Cybermancy has the effect of:  May be used as a reaction against melee attackers.</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>1416</v>
+      </c>
+      <c r="W12" t="s">
+        <v>1495</v>
+      </c>
+      <c r="X12" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/pinning-strike</v>
+      </c>
+      <c r="Y12" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/pinning-strike.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Pinning Strike in the image generation. Pinning Strike in Cybermancy has the effect of:  Pin targets limb, weapon, or clothing, restricting movement.</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1624</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/fragmentation-grenade.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>1567</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1330</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>24</v>
+      </c>
+      <c r="R13" t="s">
+        <v>25</v>
+      </c>
+      <c r="S13" t="s">
+        <v>1417</v>
+      </c>
+      <c r="T13" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/explosive</v>
+      </c>
+      <c r="U13" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/explosive.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Explosive in the image generation. Explosive in Cybermancy has the effect of:  On Hope win, half damage to all in Close range.</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>1418</v>
+      </c>
+      <c r="W13" t="s">
+        <v>1496</v>
+      </c>
+      <c r="X13" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/shrapnel-storm</v>
+      </c>
+      <c r="Y13" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/shrapnel-storm.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Shrapnel Storm in the image generation. Shrapnel Storm in Cybermancy has the effect of:  All enemies in area take full damage and mark 1 Stress.</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1625</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/emp-grenade.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>1568</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="s">
+        <v>1359</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1331</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>24</v>
+      </c>
+      <c r="R14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1419</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/disruptive</v>
+      </c>
+      <c r="U14" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/disruptive.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Disruptive in the image generation. Disruptive in Cybermancy has the effect of:  On hit, drones/tech in range must succeed or shut down 1 round.</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>1420</v>
+      </c>
+      <c r="W14" t="s">
+        <v>1498</v>
+      </c>
+      <c r="X14" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/total-system-crash</v>
+      </c>
+      <c r="Y14" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/total-system-crash.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Total System Crash in the image generation. Total System Crash in Cybermancy has the effect of:  All devices in area disabled until end of scene.</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D15" t="str">
+        <f>CONCATENATE("Cybermancy image generator thread: generate an image for ", C15, " in the size recommended by Foundry VTT for icons")</f>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/improved-monofilament-whip.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>1569</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" t="s">
+        <v>1353</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
+        <v>1355</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1332</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S15" t="s">
+        <v>1397</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/lethal-edge</v>
+      </c>
+      <c r="U15" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/lethal-edge.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Lethal Edge in the image generation. Lethal Edge in Cybermancy has the effect of:  On a Hope win, upgrade one damage die to max value.</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>1421</v>
+      </c>
+      <c r="W15" t="s">
+        <v>1500</v>
+      </c>
+      <c r="X15" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/severance</v>
+      </c>
+      <c r="Y15" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/severance.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Severance in the image generation. Severance in Cybermancy has the effect of:  Cut through armor, restraints, or environmental barriers.</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1627</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" ref="D16:D47" si="7">CONCATENATE("Cybermancy image generator thread: generate an image for ", C16, " in the size recommended by Foundry VTT for icons")</f>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/improved-cyber-spur.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16" t="s">
+        <v>1356</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1328</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>24</v>
+      </c>
+      <c r="R16" t="s">
+        <v>25</v>
+      </c>
+      <c r="S16" t="s">
+        <v>1399</v>
+      </c>
+      <c r="T16" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/concealed</v>
+      </c>
+      <c r="U16" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/concealed.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Concealed in the image generation. Concealed in Cybermancy has the effect of:  Cannot be detected by casual scans.</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>1422</v>
+      </c>
+      <c r="W16" t="s">
+        <v>1502</v>
+      </c>
+      <c r="X16" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/spinal-strike</v>
+      </c>
+      <c r="Y16" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/spinal-strike.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Spinal Strike in the image generation. Spinal Strike in Cybermancy has the effect of:  Target is paralyzed for 1 round.</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1628</v>
+      </c>
+      <c r="D17" t="str">
+        <f>CONCATENATE("Cybermancy image generator thread: generate an image for ", C17, " ", E17, " in the size recommended by Foundry VTT for icons")</f>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/improved-shock-baton.png Upgraded battery coils deliver chained electrical arcs between multiple nearby targets. in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>1571</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1357</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1326</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>24</v>
+      </c>
+      <c r="R17" t="s">
+        <v>25</v>
+      </c>
+      <c r="S17" t="s">
+        <v>1423</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/arc-charge</v>
+      </c>
+      <c r="U17" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/arc-charge.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Arc Charge in the image generation. Arc Charge in Cybermancy has the effect of:  Spend 1 Stress to arc lightning to another Very Close target.</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>1424</v>
+      </c>
+      <c r="W17" t="s">
+        <v>1504</v>
+      </c>
+      <c r="X17" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/overload</v>
+      </c>
+      <c r="Y17" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/overload.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Overload in the image generation. Overload in Cybermancy has the effect of:  Targets nervous system locks up; they drop gear.</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1629</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/improved-vibro-knife.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>1572</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1333</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>24</v>
+      </c>
+      <c r="R18" t="s">
+        <v>25</v>
+      </c>
+      <c r="S18" t="s">
+        <v>1403</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/piercing</v>
+      </c>
+      <c r="U18" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/piercing.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Piercing in the image generation. Piercing in Cybermancy has the effect of:  Ignores 1 level of armor.</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>1425</v>
+      </c>
+      <c r="W18" t="s">
+        <v>1602</v>
+      </c>
+      <c r="X18" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/assassins-cut</v>
+      </c>
+      <c r="Y18" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/assassins-cut.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Assassins Cut in the image generation. Assassins Cut in Cybermancy has the effect of:  Severe damage ignoring defenses.</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1630</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/smartpistol-mk-ii.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>1573</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1355</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1334</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>24</v>
+      </c>
+      <c r="R19" t="s">
+        <v>25</v>
+      </c>
+      <c r="S19" t="s">
+        <v>1405</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/smartlink</v>
+      </c>
+      <c r="U19" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/smartlink.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Smartlink in the image generation. Smartlink in Cybermancy has the effect of:  Auto-correct; reroll a miss once per scene.</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>1426</v>
+      </c>
+      <c r="W19" t="s">
+        <v>1506</v>
+      </c>
+      <c r="X19" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/eye-shot</v>
+      </c>
+      <c r="Y19" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/eye-shot.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Eye Shot in the image generation. Eye Shot in Cybermancy has the effect of:  Disable optics or key sensors.</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1631</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/compact-smg.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>1574</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P20" t="s">
+        <v>1335</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>24</v>
+      </c>
+      <c r="R20" t="s">
+        <v>25</v>
+      </c>
+      <c r="S20" t="s">
+        <v>1407</v>
+      </c>
+      <c r="T20" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/burst-fire</v>
+      </c>
+      <c r="U20" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/burst-fire.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Burst Fire in the image generation. Burst Fire in Cybermancy has the effect of:  Spend Hope to hit two targets in Close range.</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>1427</v>
+      </c>
+      <c r="W20" t="s">
+        <v>1508</v>
+      </c>
+      <c r="X20" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/crowd-control</v>
+      </c>
+      <c r="Y20" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/crowd-control.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Crowd Control in the image generation. Crowd Control in Cybermancy has the effect of:  Panic/disrupt all enemies in Very Close range.</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/military-assault-rifle.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" t="s">
+        <v>1336</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>24</v>
+      </c>
+      <c r="R21" t="s">
+        <v>25</v>
+      </c>
+      <c r="S21" t="s">
+        <v>1409</v>
+      </c>
+      <c r="T21" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/suppressive-fire</v>
+      </c>
+      <c r="U21" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/suppressive-fire.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Suppressive Fire in the image generation. Suppressive Fire in Cybermancy has the effect of:  On Hope win, all enemies in line of fire mark Stress.</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>1428</v>
+      </c>
+      <c r="W21" t="s">
+        <v>1510</v>
+      </c>
+      <c r="X21" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/armor-break</v>
+      </c>
+      <c r="Y21" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/armor-break.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Armor Break in the image generation. Armor Break in Cybermancy has the effect of:  Ignore armor; bullets chew through cover.</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1633</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/street-sweeper-shotgun.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>1576</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22" t="s">
+        <v>1356</v>
+      </c>
+      <c r="P22" t="s">
+        <v>1337</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>24</v>
+      </c>
+      <c r="R22" t="s">
+        <v>25</v>
+      </c>
+      <c r="S22" t="s">
+        <v>1429</v>
+      </c>
+      <c r="T22" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/wide-scatter</v>
+      </c>
+      <c r="U22" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/wide-scatter.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Wide Scatter in the image generation. Wide Scatter in Cybermancy has the effect of:  Attack all targets in Very Close range once per scene.</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>1430</v>
+      </c>
+      <c r="W22" t="s">
+        <v>1512</v>
+      </c>
+      <c r="X22" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/bone-shaker</v>
+      </c>
+      <c r="Y22" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/bone-shaker.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Bone Shaker in the image generation. Bone Shaker in Cybermancy has the effect of:  Target knocked prone and loses next turn.</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/scoped-sniper-rifle.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>1577</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" t="s">
+        <v>1354</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23" t="s">
+        <v>1359</v>
+      </c>
+      <c r="P23" t="s">
+        <v>1336</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>24</v>
+      </c>
+      <c r="R23" t="s">
+        <v>25</v>
+      </c>
+      <c r="S23" t="s">
+        <v>1413</v>
+      </c>
+      <c r="T23" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/scoped</v>
+      </c>
+      <c r="U23" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/scoped.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Scoped in the image generation. Scoped in Cybermancy has the effect of:  Aim for advantage; crit chance rises if aiming 1 round.</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="W23" t="s">
+        <v>1493</v>
+      </c>
+      <c r="X23" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/through-and-through</v>
+      </c>
+      <c r="Y23" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/through-and-through.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Through and Through in the image generation. Through and Through in Cybermancy has the effect of:  Shot penetrates multiple targets.</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/fragmentation-grenade-plus.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>1578</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" t="s">
+        <v>1337</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>24</v>
+      </c>
+      <c r="R24" t="s">
+        <v>25</v>
+      </c>
+      <c r="S24" t="s">
+        <v>1417</v>
+      </c>
+      <c r="T24" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/explosive</v>
+      </c>
+      <c r="U24" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/explosive.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Explosive in the image generation. Explosive in Cybermancy has the effect of:  Half damage to adjacent zones.</v>
+      </c>
+      <c r="V24" s="4" t="s">
+        <v>1432</v>
+      </c>
+      <c r="W24" t="s">
+        <v>1515</v>
+      </c>
+      <c r="X24" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/massive-detonation</v>
+      </c>
+      <c r="Y24" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/massive-detonation.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Massive Detonation in the image generation. Massive Detonation in Cybermancy has the effect of:  Full damage in wider zone (Far).</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/emp-grenade-plus.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>1579</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25" t="s">
+        <v>1359</v>
+      </c>
+      <c r="P25" t="s">
+        <v>1321</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>24</v>
+      </c>
+      <c r="R25" t="s">
+        <v>25</v>
+      </c>
+      <c r="S25" t="s">
+        <v>1419</v>
+      </c>
+      <c r="T25" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/disruptive</v>
+      </c>
+      <c r="U25" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/disruptive.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Disruptive in the image generation. Disruptive in Cybermancy has the effect of:  Drones/tech roll at Disadvantage.</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="W25" t="s">
+        <v>1517</v>
+      </c>
+      <c r="X25" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/grid-blackout</v>
+      </c>
+      <c r="Y25" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/grid-blackout.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Grid Blackout in the image generation. Grid Blackout in Cybermancy has the effect of:  All tech shuts down until reboot.</v>
+      </c>
+      <c r="Z25" s="4" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1635</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/corporate-mono-whip.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" t="s">
+        <v>1353</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
+        <v>1355</v>
+      </c>
+      <c r="P26" t="s">
+        <v>1338</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>24</v>
+      </c>
+      <c r="R26" t="s">
+        <v>25</v>
+      </c>
+      <c r="S26" t="s">
+        <v>1397</v>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/lethal-edge</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/lethal-edge.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Lethal Edge in the image generation. Lethal Edge in Cybermancy has the effect of:  Can slice through vehicles on Hope crit.</v>
+      </c>
+      <c r="V26" s="4" t="s">
+        <v>1434</v>
+      </c>
+      <c r="W26" t="s">
+        <v>1519</v>
+      </c>
+      <c r="X26" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/corpse-cutter</v>
+      </c>
+      <c r="Y26" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/corpse-cutter.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Corpse-Cutter in the image generation. Corpse-Cutter in Cybermancy has the effect of:  Destroy one environmental object (door, drone, wall).</v>
+      </c>
+      <c r="Z26" s="4" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1636</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/titanium-cyber-spurs.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>1581</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" t="s">
+        <v>21</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
+        <v>1356</v>
+      </c>
+      <c r="P27" t="s">
+        <v>1339</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>24</v>
+      </c>
+      <c r="R27" t="s">
+        <v>25</v>
+      </c>
+      <c r="S27" t="s">
+        <v>1435</v>
+      </c>
+      <c r="T27" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/hidden-killer</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/hidden-killer.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Hidden Killer in the image generation. Hidden Killer in Cybermancy has the effect of:  +2 to first attack in combat.</v>
+      </c>
+      <c r="V27" s="4" t="s">
+        <v>1436</v>
+      </c>
+      <c r="W27" t="s">
+        <v>1521</v>
+      </c>
+      <c r="X27" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/critical-tendons</v>
+      </c>
+      <c r="Y27" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/critical-tendons.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Critical Tendons in the image generation. Critical Tendons in Cybermancy has the effect of:  Cripple targets mobility permanently.</v>
+      </c>
+      <c r="Z27" s="4" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/heavy-shock-baton.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28" t="s">
+        <v>1357</v>
+      </c>
+      <c r="P28" t="s">
+        <v>1340</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>24</v>
+      </c>
+      <c r="R28" t="s">
+        <v>25</v>
+      </c>
+      <c r="S28" t="s">
+        <v>1437</v>
+      </c>
+      <c r="T28" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/chain-lightning</v>
+      </c>
+      <c r="U28" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/chain-lightning.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Chain Lightning in the image generation. Chain Lightning in Cybermancy has the effect of:  Spend 2 Hope, arc to 2 additional targets.</v>
+      </c>
+      <c r="V28" s="4" t="s">
+        <v>1438</v>
+      </c>
+      <c r="W28" t="s">
+        <v>1522</v>
+      </c>
+      <c r="X28" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/system-shutdown</v>
+      </c>
+      <c r="Y28" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/system-shutdown.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by System Shutdown in the image generation. System Shutdown in Cybermancy has the effect of:  Target incapacitated (stun or KO).</v>
+      </c>
+      <c r="Z28" s="4" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1638</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/combat-vibro-blade.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>1583</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P29" t="s">
+        <v>1341</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>24</v>
+      </c>
+      <c r="R29" t="s">
+        <v>25</v>
+      </c>
+      <c r="S29" t="s">
+        <v>1439</v>
+      </c>
+      <c r="T29" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/high-frequency</v>
+      </c>
+      <c r="U29" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/high-frequency.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by High Frequency in the image generation. High Frequency in Cybermancy has the effect of:  +2 to all attack rolls this scene after a hit.</v>
+      </c>
+      <c r="V29" s="4" t="s">
+        <v>1440</v>
+      </c>
+      <c r="W29" t="s">
+        <v>1524</v>
+      </c>
+      <c r="X29" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/fatal-wound</v>
+      </c>
+      <c r="Y29" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/fatal-wound.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Fatal Wound in the image generation. Fatal Wound in Cybermancy has the effect of:  Additional 1d12 bleed damage next turn.</v>
+      </c>
+      <c r="Z29" s="4" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/smartpistol-elite.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>1584</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>1355</v>
+      </c>
+      <c r="P30" t="s">
+        <v>1336</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>24</v>
+      </c>
+      <c r="R30" t="s">
+        <v>25</v>
+      </c>
+      <c r="S30" t="s">
+        <v>1441</v>
+      </c>
+      <c r="T30" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/autotarget</v>
+      </c>
+      <c r="U30" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/autotarget.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Autotarget in the image generation. Autotarget in Cybermancy has the effect of:  Always ignore cover.</v>
+      </c>
+      <c r="V30" s="4" t="s">
+        <v>1442</v>
+      </c>
+      <c r="W30" t="s">
+        <v>1526</v>
+      </c>
+      <c r="X30" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/one-shot-kill</v>
+      </c>
+      <c r="Y30" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/one-shot-kill.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by One-Shot Kill in the image generation. One-Shot Kill in Cybermancy has the effect of:  Severe damage ignoring all armor.</v>
+      </c>
+      <c r="Z30" s="4" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1640</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/advanced-smg.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>1585</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P31" t="s">
+        <v>1342</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>24</v>
+      </c>
+      <c r="R31" t="s">
+        <v>25</v>
+      </c>
+      <c r="S31" t="s">
+        <v>1443</v>
+      </c>
+      <c r="T31" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/bulletstorm</v>
+      </c>
+      <c r="U31" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/bulletstorm.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Bulletstorm in the image generation. Bulletstorm in Cybermancy has the effect of:  Once per rest, attack 3 targets in Close.</v>
+      </c>
+      <c r="V31" s="4" t="s">
+        <v>1444</v>
+      </c>
+      <c r="W31" t="s">
+        <v>1528</v>
+      </c>
+      <c r="X31" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/suppression-killzone</v>
+      </c>
+      <c r="Y31" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/suppression-killzone.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Suppression Killzone in the image generation. Suppression Killzone in Cybermancy has the effect of:  Enemies must Retreat or mark Stress.</v>
+      </c>
+      <c r="Z31" s="4" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1641</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/advanced-assault-rifle.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>1586</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M32" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" t="s">
+        <v>1343</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>24</v>
+      </c>
+      <c r="R32" t="s">
+        <v>25</v>
+      </c>
+      <c r="S32" t="s">
+        <v>1445</v>
+      </c>
+      <c r="T32" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/full-auto</v>
+      </c>
+      <c r="U32" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/full-auto.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Full Auto in the image generation. Full Auto in Cybermancy has the effect of:  Spend Hope, double damage dice.</v>
+      </c>
+      <c r="V32" s="4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="W32" t="s">
+        <v>1530</v>
+      </c>
+      <c r="X32" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/critical-barrage</v>
+      </c>
+      <c r="Y32" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/critical-barrage.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Critical Barrage in the image generation. Critical Barrage in Cybermancy has the effect of:  Mow down cover, forcing enemies into open.</v>
+      </c>
+      <c r="Z32" s="4" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1642</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/riot-shotgun.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>1587</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33" t="s">
+        <v>1356</v>
+      </c>
+      <c r="P33" t="s">
+        <v>1344</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>24</v>
+      </c>
+      <c r="R33" t="s">
+        <v>25</v>
+      </c>
+      <c r="S33" t="s">
+        <v>1447</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/knockback</v>
+      </c>
+      <c r="U33" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/knockback.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Knockback in the image generation. Knockback in Cybermancy has the effect of:  Push targets back one range band.</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>1448</v>
+      </c>
+      <c r="W33" t="s">
+        <v>1532</v>
+      </c>
+      <c r="X33" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/concussive-blast</v>
+      </c>
+      <c r="Y33" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/concussive-blast.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Concussive Blast in the image generation. Concussive Blast in Cybermancy has the effect of:  Stun all in Close cone.</v>
+      </c>
+      <c r="Z33" s="4" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1643</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/anti-materiel-sniper.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>1588</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" t="s">
+        <v>1354</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34" t="s">
+        <v>1359</v>
+      </c>
+      <c r="P34" t="s">
+        <v>1343</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>24</v>
+      </c>
+      <c r="R34" t="s">
+        <v>25</v>
+      </c>
+      <c r="S34" t="s">
+        <v>1449</v>
+      </c>
+      <c r="T34" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/penetration</v>
+      </c>
+      <c r="U34" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/penetration.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Penetration in the image generation. Penetration in Cybermancy has the effect of:  Shoot through walls/vehicles.</v>
+      </c>
+      <c r="V34" s="4" t="s">
+        <v>1450</v>
+      </c>
+      <c r="W34" t="s">
+        <v>1603</v>
+      </c>
+      <c r="X34" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/executioners-shot</v>
+      </c>
+      <c r="Y34" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/executioners-shot.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Executioners Shot in the image generation. Executioners Shot in Cybermancy has the effect of:  Instantly remove non-boss foe.</v>
+      </c>
+      <c r="Z34" s="4" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1644</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/cluster-grenade.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>1589</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35" t="s">
+        <v>22</v>
+      </c>
+      <c r="P35" t="s">
+        <v>1338</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>24</v>
+      </c>
+      <c r="R35" t="s">
+        <v>25</v>
+      </c>
+      <c r="S35" t="s">
+        <v>1451</v>
+      </c>
+      <c r="T35" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/fragment-split</v>
+      </c>
+      <c r="U35" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/fragment-split.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Fragment Split in the image generation. Fragment Split in Cybermancy has the effect of:  Hit two separate zones.</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>1452</v>
+      </c>
+      <c r="W35" t="s">
+        <v>1535</v>
+      </c>
+      <c r="X35" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/kill-zone</v>
+      </c>
+      <c r="Y35" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/kill-zone.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Kill Zone in the image generation. Kill Zone in Cybermancy has the effect of:  Full damage in all adjacent zones.</v>
+      </c>
+      <c r="Z35" s="4" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1645</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/emp-cascade.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36" t="s">
+        <v>1359</v>
+      </c>
+      <c r="P36" t="s">
+        <v>1330</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>24</v>
+      </c>
+      <c r="R36" t="s">
+        <v>25</v>
+      </c>
+      <c r="S36" t="s">
+        <v>1453</v>
+      </c>
+      <c r="T36" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/system-overload</v>
+      </c>
+      <c r="U36" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/system-overload.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by System Overload in the image generation. System Overload in Cybermancy has the effect of:  Devices take 2 rounds to recover.</v>
+      </c>
+      <c r="V36" s="4" t="s">
+        <v>1454</v>
+      </c>
+      <c r="W36" t="s">
+        <v>1537</v>
+      </c>
+      <c r="X36" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/matrix-burnout</v>
+      </c>
+      <c r="Y36" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/matrix-burnout.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Matrix Burnout in the image generation. Matrix Burnout in Cybermancy has the effect of:  Deckers hit take HP damage directly.</v>
+      </c>
+      <c r="Z36" s="4" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1646</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/legendary-monofilament-whip.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>1591</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" t="s">
+        <v>1353</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37" t="s">
+        <v>1355</v>
+      </c>
+      <c r="P37" t="s">
+        <v>1345</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>24</v>
+      </c>
+      <c r="R37" t="s">
+        <v>25</v>
+      </c>
+      <c r="S37" t="s">
+        <v>1455</v>
+      </c>
+      <c r="T37" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/reality-cut</v>
+      </c>
+      <c r="U37" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/reality-cut.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Reality Cut in the image generation. Reality Cut in Cybermancy has the effect of:  Can slice vehicles, turrets, drones.</v>
+      </c>
+      <c r="V37" s="4" t="s">
+        <v>1456</v>
+      </c>
+      <c r="W37" t="s">
+        <v>1539</v>
+      </c>
+      <c r="X37" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/sever-reality</v>
+      </c>
+      <c r="Y37" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/sever-reality.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Sever Reality in the image generation. Sever Reality in Cybermancy has the effect of:  Slice environment  create a permanent gap or hazard.</v>
+      </c>
+      <c r="Z37" s="4" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1647</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/diamond-cyber-spurs.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>1592</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" t="s">
+        <v>21</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38" t="s">
+        <v>1356</v>
+      </c>
+      <c r="P38" t="s">
+        <v>1346</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>24</v>
+      </c>
+      <c r="R38" t="s">
+        <v>25</v>
+      </c>
+      <c r="S38" t="s">
+        <v>1457</v>
+      </c>
+      <c r="T38" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/ghost-kill</v>
+      </c>
+      <c r="U38" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/ghost-kill.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Ghost Kill in the image generation. Ghost Kill in Cybermancy has the effect of:  Cannot be tracked by sensors.</v>
+      </c>
+      <c r="V38" s="4" t="s">
+        <v>1458</v>
+      </c>
+      <c r="W38" t="s">
+        <v>1540</v>
+      </c>
+      <c r="X38" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/spinal-sever</v>
+      </c>
+      <c r="Y38" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/spinal-sever.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Spinal Sever in the image generation. Spinal Sever in Cybermancy has the effect of:  Target permanently disabled unless cybernetically healed.</v>
+      </c>
+      <c r="Z38" s="4" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1648</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/thunder-baton.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>1593</v>
+      </c>
+      <c r="F39">
+        <v>4</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39" t="s">
+        <v>1357</v>
+      </c>
+      <c r="P39" t="s">
+        <v>1346</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>24</v>
+      </c>
+      <c r="R39" t="s">
+        <v>25</v>
+      </c>
+      <c r="S39" t="s">
+        <v>1459</v>
+      </c>
+      <c r="T39" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/overdrive</v>
+      </c>
+      <c r="U39" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/overdrive.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Overdrive in the image generation. Overdrive in Cybermancy has the effect of:  Once per rest, stun all enemies in Close range.</v>
+      </c>
+      <c r="V39" s="4" t="s">
+        <v>1460</v>
+      </c>
+      <c r="W39" t="s">
+        <v>1542</v>
+      </c>
+      <c r="X39" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/emp-surge</v>
+      </c>
+      <c r="Y39" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/emp-surge.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by EMP Surge in the image generation. EMP Surge in Cybermancy has the effect of:  Wipe out all small electronics in scene.</v>
+      </c>
+      <c r="Z39" s="4" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/nano-vibro-blade.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>1594</v>
+      </c>
+      <c r="F40">
+        <v>4</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40" t="s">
+        <v>20</v>
+      </c>
+      <c r="M40" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P40" t="s">
+        <v>1346</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>24</v>
+      </c>
+      <c r="R40" t="s">
+        <v>25</v>
+      </c>
+      <c r="S40" t="s">
+        <v>1461</v>
+      </c>
+      <c r="T40" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/self-sharpening</v>
+      </c>
+      <c r="U40" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/self-sharpening.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Self-Sharpening in the image generation. Self-Sharpening in Cybermancy has the effect of:  Ignore all armor values.</v>
+      </c>
+      <c r="V40" s="4" t="s">
+        <v>1462</v>
+      </c>
+      <c r="W40" t="s">
+        <v>1544</v>
+      </c>
+      <c r="X40" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/critical-dissection</v>
+      </c>
+      <c r="Y40" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/critical-dissection.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Critical Dissection in the image generation. Critical Dissection in Cybermancy has the effect of:  Narratively kill or disable any single non-boss foe.</v>
+      </c>
+      <c r="Z40" s="4" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/smartpistol-omega.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>1595</v>
+      </c>
+      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
+      </c>
+      <c r="M41" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41" t="s">
+        <v>1355</v>
+      </c>
+      <c r="P41" t="s">
+        <v>1347</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>24</v>
+      </c>
+      <c r="R41" t="s">
+        <v>25</v>
+      </c>
+      <c r="S41" t="s">
+        <v>1463</v>
+      </c>
+      <c r="T41" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/ai-assist</v>
+      </c>
+      <c r="U41" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/ai-assist.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by AI Assist in the image generation. AI Assist in Cybermancy has the effect of:  Advantage on all ranged rolls.</v>
+      </c>
+      <c r="V41" s="4" t="s">
+        <v>1464</v>
+      </c>
+      <c r="W41" t="s">
+        <v>1546</v>
+      </c>
+      <c r="X41" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/neural-kill</v>
+      </c>
+      <c r="Y41" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/neural-kill.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Neural Kill in the image generation. Neural Kill in Cybermancy has the effect of:  Bullet bypasses physical armor; deals Stress + HP.</v>
+      </c>
+      <c r="Z41" s="4" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1651</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/prototype-smg.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>1596</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
+      </c>
+      <c r="M42" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P42" t="s">
+        <v>1348</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>24</v>
+      </c>
+      <c r="R42" t="s">
+        <v>25</v>
+      </c>
+      <c r="S42" t="s">
+        <v>1465</v>
+      </c>
+      <c r="T42" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/gyrostabilized</v>
+      </c>
+      <c r="U42" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/gyrostabilized.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Gyrostabilized in the image generation. Gyrostabilized in Cybermancy has the effect of:  Fire with no recoil penalty.</v>
+      </c>
+      <c r="V42" s="4" t="s">
+        <v>1466</v>
+      </c>
+      <c r="W42" t="s">
+        <v>1548</v>
+      </c>
+      <c r="X42" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/critical-spray</v>
+      </c>
+      <c r="Y42" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/critical-spray.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Critical Spray in the image generation. Critical Spray in Cybermancy has the effect of:  Hit all enemies in Close range automatically.</v>
+      </c>
+      <c r="Z42" s="4" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" ht="58" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/gauss-rifle.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>1597</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
+      </c>
+      <c r="M43" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43" t="s">
+        <v>22</v>
+      </c>
+      <c r="P43" t="s">
+        <v>1349</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>24</v>
+      </c>
+      <c r="R43" t="s">
+        <v>25</v>
+      </c>
+      <c r="S43" t="s">
+        <v>1467</v>
+      </c>
+      <c r="T43" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/rail-shot</v>
+      </c>
+      <c r="U43" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/rail-shot.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Rail Shot in the image generation. Rail Shot in Cybermancy has the effect of:  Spend Stress to deal double damage dice.</v>
+      </c>
+      <c r="V43" s="4" t="s">
+        <v>1468</v>
+      </c>
+      <c r="W43" t="s">
+        <v>1550</v>
+      </c>
+      <c r="X43" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/hyper-pierce</v>
+      </c>
+      <c r="Y43" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/hyper-pierce.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Hyper-Pierce in the image generation. Hyper-Pierce in Cybermancy has the effect of:  Shot tears through multiple enemies/vehicles in a line.</v>
+      </c>
+      <c r="Z43" s="4" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1653</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/plasma-shotgun.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>1598</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" t="s">
+        <v>20</v>
+      </c>
+      <c r="M44" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44" t="s">
+        <v>1356</v>
+      </c>
+      <c r="P44" t="s">
+        <v>1349</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>24</v>
+      </c>
+      <c r="R44" t="s">
+        <v>25</v>
+      </c>
+      <c r="S44" t="s">
+        <v>1469</v>
+      </c>
+      <c r="T44" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/meltdown</v>
+      </c>
+      <c r="U44" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/meltdown.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Meltdown in the image generation. Meltdown in Cybermancy has the effect of:  Spend Hope to add 1d8 burn damage.</v>
+      </c>
+      <c r="V44" s="4" t="s">
+        <v>1470</v>
+      </c>
+      <c r="W44" t="s">
+        <v>1552</v>
+      </c>
+      <c r="X44" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/critical-inferno</v>
+      </c>
+      <c r="Y44" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/critical-inferno.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Critical Inferno in the image generation. Critical Inferno in Cybermancy has the effect of:  All targets in blast zone catch fire.</v>
+      </c>
+      <c r="Z44" s="4" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1654</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/orbital-sniper-rifle.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>1599</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" t="s">
+        <v>20</v>
+      </c>
+      <c r="M45" t="s">
+        <v>1354</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45" t="s">
+        <v>1359</v>
+      </c>
+      <c r="P45" t="s">
+        <v>1349</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>24</v>
+      </c>
+      <c r="R45" t="s">
+        <v>25</v>
+      </c>
+      <c r="S45" t="s">
+        <v>1471</v>
+      </c>
+      <c r="T45" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/satellite-link</v>
+      </c>
+      <c r="U45" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/satellite-link.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Satellite Link in the image generation. Satellite Link in Cybermancy has the effect of:  Call in orbital fire once per rest.</v>
+      </c>
+      <c r="V45" s="4" t="s">
+        <v>1472</v>
+      </c>
+      <c r="W45" t="s">
+        <v>1607</v>
+      </c>
+      <c r="X45" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/heavens-lance</v>
+      </c>
+      <c r="Y45" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/heavens-lance.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Heavens Lance in the image generation. Heavens Lance in Cybermancy has the effect of:  Obliterate target zone, GM narrates consequences.</v>
+      </c>
+      <c r="Z45" s="4" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/annihilation-grenade.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" t="s">
+        <v>20</v>
+      </c>
+      <c r="M46" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46" t="s">
+        <v>22</v>
+      </c>
+      <c r="P46" t="s">
+        <v>1350</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>24</v>
+      </c>
+      <c r="R46" t="s">
+        <v>25</v>
+      </c>
+      <c r="S46" t="s">
+        <v>1473</v>
+      </c>
+      <c r="T46" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/final-boom</v>
+      </c>
+      <c r="U46" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/final-boom.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Final Boom in the image generation. Final Boom in Cybermancy has the effect of:  Single-use, but massive radius.</v>
+      </c>
+      <c r="V46" s="4" t="s">
+        <v>1474</v>
+      </c>
+      <c r="W46" t="s">
+        <v>1554</v>
+      </c>
+      <c r="X46" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/tactical-nuke-(micro)</v>
+      </c>
+      <c r="Y46" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/tactical-nuke-(micro).png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Tactical Nuke (Micro) in the image generation. Tactical Nuke (Micro) in Cybermancy has the effect of:  Entire area wiped  citywide consequences.</v>
+      </c>
+      <c r="Z46" s="4" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1656</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="7"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons/emp-singularity.png in the size recommended by Foundry VTT for icons</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F47">
+        <v>4</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" t="s">
+        <v>27</v>
+      </c>
+      <c r="I47" t="s">
+        <v>20</v>
+      </c>
+      <c r="M47" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47" t="s">
+        <v>1359</v>
+      </c>
+      <c r="P47" t="s">
+        <v>1350</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>24</v>
+      </c>
+      <c r="R47" t="s">
+        <v>25</v>
+      </c>
+      <c r="S47" t="s">
+        <v>1475</v>
+      </c>
+      <c r="T47" t="str">
+        <f t="shared" si="6"/>
+        <v>modules/cybermancy/assets/icons/weapons-feature/blackout</v>
+      </c>
+      <c r="U47" t="str">
+        <f t="shared" si="1"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/weapons-feature/blackout.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by Blackout in the image generation. Blackout in Cybermancy has the effect of:  Kill power grid in 1 km radius once per rest.</v>
+      </c>
+      <c r="V47" s="4" t="s">
+        <v>1476</v>
+      </c>
+      <c r="W47" t="s">
+        <v>1555</v>
+      </c>
+      <c r="X47" t="str">
+        <f t="shared" si="4"/>
+        <v>modules/cybermancy/assets/icons/features/system-collapse</v>
+      </c>
+      <c r="Y47" t="str">
+        <f t="shared" si="5"/>
+        <v>Cybermancy image generator thread: generate an image for modules/cybermancy/assets/icons/features/system-collapse.png in the size recommended by Foundry VTT for icons.  Focus on the descriptive aspects implied by System Collapse in the image generation. System Collapse in Cybermancy has the effect of:  Entire Matrix zone crashes beyond repair.</v>
+      </c>
+      <c r="Z47" s="4" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{914DC4EC-A891-435E-AD2A-76436998A8C7}">
+      <formula1>1</formula1>
+      <formula2>4</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;10&amp;K000000 Revvity Proprietary Information</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E3466477-CEDE-4560-9CEE-D928858E09B2}">
+          <x14:formula1>
+            <xm:f>'Controlled Lists'!$H$2:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2:Q1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4E89FD5-FE25-4CFB-A918-FD22073EDC6E}">
+          <x14:formula1>
+            <xm:f>'Controlled Lists'!$I$2:$I$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2:R1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C03F2E2C-FEEA-4D76-AD53-54682C78D9BF}">
+          <x14:formula1>
+            <xm:f>'Controlled Lists'!$F$2:$F$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B078C6EA-DC82-4C08-8677-EAF96D0C98A3}">
+          <x14:formula1>
+            <xm:f>'Controlled Lists'!$K$2:$K$49</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4F369775-DDF2-47A3-800D-EF83EF2F8563}">
+          <x14:formula1>
+            <xm:f>'Actions and Effects'!$B:$B</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:K1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E686D192-2305-4189-A649-5A945B43EECE}">
+          <x14:formula1>
+            <xm:f>'Controlled Lists'!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02895020-FC90-4395-A540-A8C55B3381CB}">
+          <x14:formula1>
+            <xm:f>'Controlled Lists'!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2231F62D-7182-49A5-A170-8043111B0E34}">
+          <x14:formula1>
+            <xm:f>'Controlled Lists'!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A0210F-6AD5-4290-AC2A-0367F956D048}">
   <dimension ref="A1:K49"/>
   <sheetViews>
@@ -9083,7 +12786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E888BC-20E7-4294-8A2D-BD0A7B31655F}">
   <dimension ref="A1:E530"/>
   <sheetViews>
@@ -18118,11 +21821,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA33895-3184-47ED-9CD0-40CC7512F6C6}">
   <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -18389,375 +22092,212 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8134B3E0-0F30-40E4-A4E1-00A26E5811E5}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="106.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>0</v>
+        <v>1662</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="232" x14ac:dyDescent="0.35">
+        <v>1663</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>1276</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
-        <v>1277</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>1558</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>1278</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>1559</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>1279</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>1280</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>1281</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>1563</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
-        <v>1284</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="145" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
-        <v>1285</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>1566</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="145" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>1286</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>1567</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>1287</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="203" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>1288</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="203" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>1290</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>1291</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="145" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
-        <v>1292</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
-        <v>1293</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
-        <v>1294</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>1296</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>1578</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
-        <v>1298</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>1579</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
-        <v>1299</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>1300</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>1581</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
-        <v>1301</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>1582</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
-        <v>1302</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="145" x14ac:dyDescent="0.35">
-      <c r="A29" s="10" t="s">
-        <v>1303</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
-        <v>1304</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="145" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
-        <v>1305</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>1586</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
-        <v>1306</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
-        <v>1307</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
-        <v>1308</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
-        <v>1309</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A36" s="10" t="s">
-        <v>1310</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A37" s="10" t="s">
-        <v>1311</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A38" s="10" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
-        <v>1313</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="10" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>1595</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="10" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>1596</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="10" t="s">
-        <v>1316</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A43" s="10" t="s">
-        <v>1317</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>1598</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A44" s="10" t="s">
-        <v>1318</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>1599</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="145" x14ac:dyDescent="0.35">
-      <c r="A45" s="10" t="s">
-        <v>1319</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>1600</v>
-      </c>
+        <v>1666</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="10"/>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="10"/>
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="10"/>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="10"/>
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="10"/>
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="10"/>
+      <c r="B27" s="9"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="10"/>
+      <c r="B28" s="9"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="9"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="10"/>
+      <c r="B30" s="9"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="10"/>
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="10"/>
+      <c r="B32" s="9"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="9"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="10"/>
+      <c r="B35" s="9"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="10"/>
+      <c r="B36" s="9"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="10"/>
+      <c r="B38" s="9"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="10"/>
+      <c r="B40" s="9"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="10"/>
+      <c r="B42" s="9"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="10"/>
+      <c r="B43" s="9"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="10"/>
+      <c r="B44" s="9"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="10"/>
+      <c r="B45" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished the first review of the loot and consumables.  Started work on first adventure
</commit_message>
<xml_diff>
--- a/pyCybermancy/cybermancy-object-list.xlsx
+++ b/pyCybermancy/cybermancy-object-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Daniel\role-gaming\Cybermancy module development\cybermancy\pyCybermancy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD9A12B-EDF6-41CD-8C93-49F4443F0CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E31AA1-0D61-4947-ABD8-26CBFCE73139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="20565" windowWidth="29040" windowHeight="15720" tabRatio="777" firstSheet="2" activeTab="11" xr2:uid="{15A82952-0862-46EA-9957-B8D36A030377}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="777" firstSheet="2" activeTab="13" xr2:uid="{15A82952-0862-46EA-9957-B8D36A030377}"/>
   </bookViews>
   <sheets>
     <sheet name="weapons" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7962" uniqueCount="3901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7989" uniqueCount="3921">
   <si>
     <t>name</t>
   </si>
@@ -12733,6 +12733,66 @@
   </si>
   <si>
     <t>Your Primary Drone gains the ability to deploy a linear barrier.  Any creature can gain the Hidden condition by crouching down behind the barrier, but the drone may now gain the Hidden condition from its own portable barrier.</t>
+  </si>
+  <si>
+    <t>attack.name</t>
+  </si>
+  <si>
+    <t>attack.damage</t>
+  </si>
+  <si>
+    <t>experienceName</t>
+  </si>
+  <si>
+    <t>experienceBonus</t>
+  </si>
+  <si>
+    <t>attack.img</t>
+  </si>
+  <si>
+    <t>Choir of Glass knifer</t>
+  </si>
+  <si>
+    <t>Carries a shard knife, low-end AR visor, and a pocket speaker that emits disorienting tones.</t>
+  </si>
+  <si>
+    <t>harass, intimidate, threaten, convert</t>
+  </si>
+  <si>
+    <t>Stab</t>
+  </si>
+  <si>
+    <t>1d6+1</t>
+  </si>
+  <si>
+    <t>Religious argument</t>
+  </si>
+  <si>
+    <t>adversary</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>system.description</t>
+  </si>
+  <si>
+    <t>system.tier</t>
+  </si>
+  <si>
+    <t>system.motivesAndTactics</t>
+  </si>
+  <si>
+    <t>system.notes</t>
+  </si>
+  <si>
+    <t>system.difficulty</t>
+  </si>
+  <si>
+    <t>system.damageThresholds.majorThreshold</t>
+  </si>
+  <si>
+    <t>system.damageThresholds.severeThreshold</t>
   </si>
 </sst>
 </file>
@@ -27304,7 +27364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505CFBCA-2C2D-462D-87B0-C470CF4E2D4D}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD51"/>
     </sheetView>
   </sheetViews>
@@ -30003,12 +30063,137 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3452830-8D2F-4382-81BA-07482F749090}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="19.90625" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="30.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3914</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2945</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3915</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3917</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3916</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3918</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3919</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3920</v>
+      </c>
+      <c r="O1" t="s">
+        <v>3901</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3902</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3905</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3903</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3906</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3912</v>
+      </c>
+      <c r="C2" t="str">
+        <f>LOWER(SUBSTITUTE(A2, " ", "-"))</f>
+        <v>choir-of-glass-knifer</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3907</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3913</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3908</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3909</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3910</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>LOWER(SUBSTITUTE(O2," ", "-"))</f>
+        <v>stab</v>
+      </c>
+      <c r="R2" t="s">
+        <v>3911</v>
+      </c>
+      <c r="S2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
First player characters build and page add to docs to serve them up.  Also all Adversaries done.
</commit_message>
<xml_diff>
--- a/pyCybermancy/cybermancy-object-list.xlsx
+++ b/pyCybermancy/cybermancy-object-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Daniel\role-gaming\Cybermancy module development\cybermancy\pyCybermancy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E31AA1-0D61-4947-ABD8-26CBFCE73139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA226C7-0DA7-4AD4-8A03-5AE2EA52530F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="777" firstSheet="2" activeTab="13" xr2:uid="{15A82952-0862-46EA-9957-B8D36A030377}"/>
+    <workbookView xWindow="57480" yWindow="20565" windowWidth="29040" windowHeight="15720" tabRatio="777" firstSheet="2" activeTab="13" xr2:uid="{15A82952-0862-46EA-9957-B8D36A030377}"/>
   </bookViews>
   <sheets>
     <sheet name="weapons" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7989" uniqueCount="3921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8033" uniqueCount="3956">
   <si>
     <t>name</t>
   </si>
@@ -12735,21 +12735,12 @@
     <t>Your Primary Drone gains the ability to deploy a linear barrier.  Any creature can gain the Hidden condition by crouching down behind the barrier, but the drone may now gain the Hidden condition from its own portable barrier.</t>
   </si>
   <si>
-    <t>attack.name</t>
-  </si>
-  <si>
-    <t>attack.damage</t>
-  </si>
-  <si>
     <t>experienceName</t>
   </si>
   <si>
     <t>experienceBonus</t>
   </si>
   <si>
-    <t>attack.img</t>
-  </si>
-  <si>
     <t>Choir of Glass knifer</t>
   </si>
   <si>
@@ -12774,25 +12765,139 @@
     <t>standard</t>
   </si>
   <si>
-    <t>system.description</t>
-  </si>
-  <si>
-    <t>system.tier</t>
-  </si>
-  <si>
-    <t>system.motivesAndTactics</t>
-  </si>
-  <si>
-    <t>system.notes</t>
-  </si>
-  <si>
-    <t>system.difficulty</t>
-  </si>
-  <si>
-    <t>system.damageThresholds.majorThreshold</t>
-  </si>
-  <si>
-    <t>system.damageThresholds.severeThreshold</t>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>motivesAndTactics</t>
+  </si>
+  <si>
+    <t>difficulty</t>
+  </si>
+  <si>
+    <t>majorThreshold</t>
+  </si>
+  <si>
+    <t>severeThreshold</t>
+  </si>
+  <si>
+    <t>He slashes at you with a glass knife</t>
+  </si>
+  <si>
+    <t>attackBonus</t>
+  </si>
+  <si>
+    <t>attackName</t>
+  </si>
+  <si>
+    <t>attackDescription</t>
+  </si>
+  <si>
+    <t>attackDamage</t>
+  </si>
+  <si>
+    <t>attackRange</t>
+  </si>
+  <si>
+    <t>attackImg</t>
+  </si>
+  <si>
+    <t>systemType</t>
+  </si>
+  <si>
+    <t>Glassmask Lookout</t>
+  </si>
+  <si>
+    <t>Rave Enforcer</t>
+  </si>
+  <si>
+    <t>Echo Runner</t>
+  </si>
+  <si>
+    <t>Pattern-Touched Beggar</t>
+  </si>
+  <si>
+    <t>skulk</t>
+  </si>
+  <si>
+    <t>bruiser</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>ranged</t>
+  </si>
+  <si>
+    <t>hide, flank, divide, profit, escape</t>
+  </si>
+  <si>
+    <t>Wears a cracked, reflective faceplate that hides identity and displays looping memetic patterns. Uses a cheap pistol and a signal whistle tied to Abraxas-pattern frequencies.</t>
+  </si>
+  <si>
+    <t>Implanted subdermal LEDs pulse with hypnotic rhythm. Swings a reinforced baton synchronized to their internal beat-generator.</t>
+  </si>
+  <si>
+    <t>Constant noise maker in combat.  Drops a beat and then beats on you</t>
+  </si>
+  <si>
+    <t>Unpredictable, mumbling fragments of pattern phrases. Carries improvised weapons. Presence causes mild psychic static in their vicinity.</t>
+  </si>
+  <si>
+    <t>confuse, disorient, convert, suborn</t>
+  </si>
+  <si>
+    <t>intimidate, bully, steal, protect</t>
+  </si>
+  <si>
+    <t>harass, confuse, dance, mobility, escape</t>
+  </si>
+  <si>
+    <t>Heavy Pistol</t>
+  </si>
+  <si>
+    <t>Crowbar</t>
+  </si>
+  <si>
+    <t>Sonic Blast</t>
+  </si>
+  <si>
+    <t>Psychic Distrubance</t>
+  </si>
+  <si>
+    <t>Shots fired!</t>
+  </si>
+  <si>
+    <t>This is not what the crowbar was meant for!</t>
+  </si>
+  <si>
+    <t>A disorienting rush of sound</t>
+  </si>
+  <si>
+    <t>Your brain is squeezed from the inside</t>
+  </si>
+  <si>
+    <t>1d6+2</t>
+  </si>
+  <si>
+    <t>1d8</t>
+  </si>
+  <si>
+    <t>1d10+3</t>
+  </si>
+  <si>
+    <t>1d4+2</t>
+  </si>
+  <si>
+    <t>Backstab</t>
+  </si>
+  <si>
+    <t>Unveiled Threats</t>
+  </si>
+  <si>
+    <t>Cacophony</t>
+  </si>
+  <si>
+    <t>Resonance Knowledge</t>
   </si>
 </sst>
 </file>
@@ -30063,20 +30168,21 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3452830-8D2F-4382-81BA-07482F749090}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
     <col min="3" max="3" width="19.90625" customWidth="1"/>
     <col min="4" max="4" width="26.1796875" customWidth="1"/>
     <col min="8" max="8" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -30087,19 +30193,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3914</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2945</v>
+        <v>3923</v>
       </c>
       <c r="F1" t="s">
-        <v>3915</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>3917</v>
+        <v>3911</v>
       </c>
       <c r="H1" t="s">
-        <v>3916</v>
+        <v>3912</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
@@ -30108,93 +30214,362 @@
         <v>42</v>
       </c>
       <c r="K1" t="s">
+        <v>3913</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3917</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3914</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3915</v>
+      </c>
+      <c r="O1" t="s">
         <v>3918</v>
       </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>3919</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>3920</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
+        <v>3921</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3922</v>
+      </c>
+      <c r="T1" t="s">
         <v>3901</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>3902</v>
       </c>
-      <c r="Q1" t="s">
-        <v>3905</v>
-      </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3903</v>
       </c>
-      <c r="S1" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3906</v>
-      </c>
       <c r="B2" t="s">
-        <v>3912</v>
+        <v>3909</v>
       </c>
       <c r="C2" t="str">
         <f>LOWER(SUBSTITUTE(A2, " ", "-"))</f>
         <v>choir-of-glass-knifer</v>
       </c>
       <c r="D2" t="s">
-        <v>3907</v>
+        <v>3904</v>
       </c>
       <c r="E2" t="s">
-        <v>3913</v>
+        <v>3910</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>3908</v>
+        <v>3905</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>3909</v>
+        <v>3906</v>
       </c>
       <c r="P2" t="s">
-        <v>3910</v>
-      </c>
-      <c r="Q2" t="str">
+        <v>3916</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3948</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="str">
         <f>LOWER(SUBSTITUTE(O2," ", "-"))</f>
         <v>stab</v>
       </c>
-      <c r="R2" t="s">
-        <v>3911</v>
-      </c>
-      <c r="S2">
+      <c r="T2" t="s">
+        <v>3908</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3924</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3909</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C6" si="0">LOWER(SUBSTITUTE(A3, " ", "-"))</f>
+        <v>glassmask-lookout</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3933</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3928</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3932</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>11</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3940</v>
+      </c>
+      <c r="P3" t="s">
+        <v>3944</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>3949</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S6" si="1">LOWER(SUBSTITUTE(O3," ", "-"))</f>
+        <v>heavy-pistol</v>
+      </c>
+      <c r="T3" t="s">
+        <v>3952</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3925</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3909</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>rave-enforcer</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3934</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3929</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3938</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
         <v>3</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3941</v>
+      </c>
+      <c r="P4" t="s">
+        <v>3945</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>3950</v>
+      </c>
+      <c r="R4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="1"/>
+        <v>crowbar</v>
+      </c>
+      <c r="T4" t="s">
+        <v>3953</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3926</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3909</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>echo-runner</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3935</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3930</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3939</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
+        <v>3942</v>
+      </c>
+      <c r="P5" t="s">
+        <v>3946</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>3951</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" si="1"/>
+        <v>sonic-blast</v>
+      </c>
+      <c r="T5" t="s">
+        <v>3954</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3927</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3909</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>pattern-touched-beggar</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3936</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3931</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3937</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>9</v>
+      </c>
+      <c r="O6" t="s">
+        <v>3943</v>
+      </c>
+      <c r="P6" t="s">
+        <v>3947</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>3907</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1352</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="1"/>
+        <v>psychic-distrubance</v>
+      </c>
+      <c r="T6" t="s">
+        <v>3955</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>